<commit_message>
feat: implement geographical distribution for household bio
</commit_message>
<xml_diff>
--- a/ebm/geografisk_inndeling/data/fjernvarme_kommune_fordelingsnøkler.xlsx
+++ b/ebm/geografisk_inndeling/data/fjernvarme_kommune_fordelingsnøkler.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nveazure-my.sharepoint.com/personal/moe_nve_no/Documents/prosjekter/Geografisk_inndeling_EBM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="562" documentId="8_{A264A099-37C8-461C-B91F-B4D99187099B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{73C2780E-1093-4CE8-B065-41DABEB291D6}"/>
+  <xr:revisionPtr revIDLastSave="563" documentId="8_{A264A099-37C8-461C-B91F-B4D99187099B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5B6A15A3-9B04-4439-9BBC-C2B4E10AC51E}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-870" windowWidth="29040" windowHeight="17520" xr2:uid="{231E4ED5-222D-4157-8B6F-4EFA2FA515C6}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{231E4ED5-222D-4157-8B6F-4EFA2FA515C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -845,13 +845,13 @@
     <t>5622</t>
   </si>
   <si>
-    <t>9999</t>
-  </si>
-  <si>
     <t>bolig</t>
   </si>
   <si>
     <t>yrkesbygg</t>
+  </si>
+  <si>
+    <t>2100</t>
   </si>
 </sst>
 </file>
@@ -1267,8 +1267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{789F07F8-EEE9-42A4-94C2-85B405DA6A62}">
   <dimension ref="A1:I358"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="G135" sqref="G135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1287,10 +1287,10 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D1" t="s">
         <v>270</v>
-      </c>
-      <c r="D1" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -3198,7 +3198,7 @@
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" s="4" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B135" s="7" t="s">
         <v>246</v>

</xml_diff>